<commit_message>
Processing Hollis data, 3-layer-model with SD on observations
</commit_message>
<xml_diff>
--- a/data/raw/Eocene/Hollis2019SI/Hollis2019_d18O_locations.xlsx
+++ b/data/raw/Eocene/Hollis2019SI/Hollis2019_d18O_locations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PalaeoClimateGradient\data\raw\Eocene\Hollis2019SI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F70054-A93B-414F-BD13-6E75D53DFF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC656826-8B91-4974-8E42-F227E05F0202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3091D935-901D-4887-B397-A4352051D1D5}"/>
+    <workbookView xWindow="4320" yWindow="3495" windowWidth="21600" windowHeight="11385" xr2:uid="{3091D935-901D-4887-B397-A4352051D1D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2836B4-D4C2-4500-8989-F059700D00FB}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,7 +1137,7 @@
         <v>-45.32</v>
       </c>
       <c r="D19">
-        <v>107.83</v>
+        <v>170.83</v>
       </c>
       <c r="E19">
         <v>-48.22</v>

</xml_diff>